<commit_message>
1. add configs submodule; 2. several improvements from document improvements.
</commit_message>
<xml_diff>
--- a/exampleTables/exampleData.xlsx
+++ b/exampleTables/exampleData.xlsx
@@ -1,34 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DocsHDD\configs\exampleTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DocsHDD\FGame\中鱼\StatDemo\exampleTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD856EC-675B-4FEE-AA17-029FF1472703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C2CE69-9760-4E16-8C84-F791A4E8AD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="765" windowWidth="34530" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="0" windowWidth="31575" windowHeight="20985" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material" sheetId="1" r:id="rId1"/>
     <sheet name="bait" sheetId="6" r:id="rId2"/>
-    <sheet name="pond" sheetId="4" r:id="rId3"/>
-    <sheet name="environment" sheetId="2" r:id="rId4"/>
+    <sheet name="baitSubType" sheetId="8" r:id="rId3"/>
+    <sheet name="baitId" sheetId="9" r:id="rId4"/>
+    <sheet name="minCoeffThld" sheetId="10" r:id="rId5"/>
+    <sheet name="environment" sheetId="2" r:id="rId6"/>
+    <sheet name="pond" sheetId="4" r:id="rId7"/>
+    <sheet name="饵subType示意" sheetId="11" r:id="rId8"/>
+    <sheet name="feed_waterlayer" sheetId="7" r:id="rId9"/>
+    <sheet name="饵Id亲和调整示意" sheetId="12" r:id="rId10"/>
+    <sheet name="水温示意" sheetId="13" r:id="rId11"/>
+    <sheet name="Weather示意" sheetId="14" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>Water</t>
   </si>
@@ -140,6 +159,231 @@
   </si>
   <si>
     <t>小型旋转亮片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼种</t>
+  </si>
+  <si>
+    <t>表层亲和系数</t>
+  </si>
+  <si>
+    <t>中层亲和系数</t>
+  </si>
+  <si>
+    <t>底层亲和系数</t>
+  </si>
+  <si>
+    <t>活虫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淀粉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>环境系数最小阈值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>适配系数最小阈值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水牛鱼-幼小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金鲈-普通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小冠太阳鱼-普通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>环境系数最小阈值</t>
+  </si>
+  <si>
+    <t>适配系数最小阈值</t>
+  </si>
+  <si>
+    <t>鱼种</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水牛鱼-普通</t>
+  </si>
+  <si>
+    <t>黄金鲈-奖杯</t>
+  </si>
+  <si>
+    <t>黄金鲈-奖杯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饵subType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亲和度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谷物</t>
+  </si>
+  <si>
+    <t>面饵</t>
+  </si>
+  <si>
+    <t>软体动物</t>
+  </si>
+  <si>
+    <t>昆虫</t>
+  </si>
+  <si>
+    <t>米诺型</t>
+  </si>
+  <si>
+    <t>波扒型</t>
+  </si>
+  <si>
+    <t>亮片型</t>
+  </si>
+  <si>
+    <t>软饵型</t>
+  </si>
+  <si>
+    <t>昆虫类</t>
+  </si>
+  <si>
+    <t>蚯蚓类</t>
+  </si>
+  <si>
+    <t>面包虫类</t>
+  </si>
+  <si>
+    <t>饵名</t>
+  </si>
+  <si>
+    <t>调整值</t>
+  </si>
+  <si>
+    <t>玉米粒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发酵玉米</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜂蜜面团</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金属光泽米诺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荧光波帕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小冠太阳鱼-普通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活蜻蜓幼虫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唯一值</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>天气名称</t>
+  </si>
+  <si>
+    <t>气温范围MIN (0.1摄氏度)</t>
+  </si>
+  <si>
+    <t>气温范围MAX (0.1摄氏度)</t>
+  </si>
+  <si>
+    <t>风速范围MIN (0.1米)</t>
+  </si>
+  <si>
+    <t>风速范围MAX  (0.1米)</t>
+  </si>
+  <si>
+    <t>最低温度 (0.1摄氏度)</t>
+  </si>
+  <si>
+    <t>最高温度 (0.1摄氏度)</t>
+  </si>
+  <si>
+    <t>相对湿度（百分比）</t>
+  </si>
+  <si>
+    <t>风向</t>
+  </si>
+  <si>
+    <t>[OutTemp]#1</t>
+  </si>
+  <si>
+    <t>[OutTemp]#2</t>
+  </si>
+  <si>
+    <t>[WindSpeed]#1</t>
+  </si>
+  <si>
+    <t>[WindSpeed]#2</t>
+  </si>
+  <si>
+    <t>[WaterTemp]#1</t>
+  </si>
+  <si>
+    <t>[WaterTemp]#2</t>
+  </si>
+  <si>
+    <t>weather_weight1</t>
+  </si>
+  <si>
+    <t>weather_sunny</t>
+  </si>
+  <si>
+    <t>[风向]东</t>
+  </si>
+  <si>
+    <t>weather_weight2</t>
+  </si>
+  <si>
+    <t>[风向]北</t>
+  </si>
+  <si>
+    <t>表层水温</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -147,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,16 +432,82 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -233,11 +543,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -258,11 +594,95 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -541,7 +961,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -649,13 +1069,429 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7DFAE5-AB60-4411-B1B6-E18E891DF574}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>0.05</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12811417-E1D7-4E73-9AAB-8C645EDDEEB7}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>18.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>23.5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E30EAD9-5764-40D2-BC68-89572CF4650C}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
+        <v>201230001</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="19">
+        <v>200</v>
+      </c>
+      <c r="E3" s="19">
+        <v>230</v>
+      </c>
+      <c r="F3" s="19">
+        <v>10</v>
+      </c>
+      <c r="G3" s="19">
+        <v>12</v>
+      </c>
+      <c r="H3" s="19">
+        <v>150</v>
+      </c>
+      <c r="I3" s="19">
+        <v>180</v>
+      </c>
+      <c r="J3" s="19">
+        <v>32</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <v>201230002</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="19">
+        <v>230</v>
+      </c>
+      <c r="E4" s="19">
+        <v>260</v>
+      </c>
+      <c r="F4" s="19">
+        <v>12</v>
+      </c>
+      <c r="G4" s="19">
+        <v>14</v>
+      </c>
+      <c r="H4" s="19">
+        <v>180</v>
+      </c>
+      <c r="I4" s="19">
+        <v>210</v>
+      </c>
+      <c r="J4" s="19">
+        <v>32</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" s="21">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A2">
+    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B2">
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="B1:B2" xr:uid="{0D8FE403-D93E-4845-BB61-5772B90596E8}">
+      <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
+    </dataValidation>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="A1:A4" xr:uid="{3432645A-AE40-40B7-8601-F67FDB6C9B32}">
+      <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3B4906-9898-4C94-BEC7-7D51CF33D9A9}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -880,47 +1716,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86CADA1-99EA-4E5D-B331-40E90BFA26D1}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B3B6C8-7450-4A15-8449-29BC50286675}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>500</v>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -930,12 +1774,131 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AECEE1-717B-48BF-9F04-EA7DFBBF8AFA}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B824A00-FEF9-4B60-8939-3C1559D1BAF4}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C20722B-E7BB-42C9-B1E1-980A6E2FAF49}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="C4" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1026,4 +1989,321 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86CADA1-99EA-4E5D-B331-40E90BFA26D1}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>800</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A236B3-3EEF-4290-A80D-BFAB0B7C23E6}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C16BDF-42F8-4ED1-A4FB-6BD61DA7AA09}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>